<commit_message>
Check Win is done
</commit_message>
<xml_diff>
--- a/files/Fight Club.xlsx
+++ b/files/Fight Club.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dexter\Desktop\Senior-Project\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dexter Miller\Desktop\Senior-Project\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D433D1F7-50BC-40E9-8EA2-57507D02D353}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A097A9E1-6129-45CC-AE19-A9EB9EA60D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="735" windowWidth="22140" windowHeight="13200" activeTab="1" xr2:uid="{05B69504-E768-412D-824E-3515363319EF}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{05B69504-E768-412D-824E-3515363319EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Wk 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>FightClub!</t>
   </si>
@@ -564,13 +564,13 @@
       <selection activeCell="B6" sqref="A1:I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.41015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="C2" s="1">
         <v>43895</v>
       </c>
@@ -604,7 +604,7 @@
         <v>43901</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
@@ -627,7 +627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -641,7 +641,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
         <v>1</v>
@@ -653,7 +653,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -664,7 +664,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="8"/>
       <c r="B7" t="s">
         <v>6</v>
@@ -673,7 +673,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="8"/>
       <c r="B8" t="s">
         <v>7</v>
@@ -681,7 +681,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
@@ -695,7 +695,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" s="8"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -710,7 +710,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" s="8"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -725,7 +725,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="8"/>
       <c r="B12" t="s">
         <v>12</v>
@@ -740,7 +740,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -765,7 +765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="8"/>
       <c r="B15" t="s">
         <v>17</v>
@@ -774,7 +774,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -785,7 +785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="8"/>
       <c r="B17" t="s">
         <v>21</v>
@@ -794,7 +794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
@@ -805,7 +805,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="8"/>
       <c r="B19" t="s">
         <v>23</v>
@@ -814,7 +814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" s="8"/>
       <c r="B20" t="s">
         <v>24</v>
@@ -846,16 +846,16 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="C2" s="1">
         <v>43895</v>
       </c>
@@ -889,7 +889,7 @@
         <v>43901</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
@@ -912,7 +912,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -926,7 +926,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B5" s="9"/>
       <c r="C5" s="7" t="s">
         <v>1</v>
@@ -938,7 +938,7 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -953,7 +953,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
@@ -963,7 +963,9 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G7" s="5" t="s">
         <v>42</v>
       </c>
@@ -974,7 +976,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="8"/>
       <c r="B8" t="s">
         <v>11</v>
@@ -982,7 +984,9 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G8" s="5" t="s">
         <v>42</v>
       </c>
@@ -993,7 +997,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="8"/>
       <c r="B9" t="s">
         <v>41</v>
@@ -1001,7 +1005,9 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="G9" s="5" t="s">
         <v>42</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="8"/>
       <c r="B10" t="s">
         <v>35</v>
@@ -1025,7 +1031,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1040,7 +1046,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
@@ -1055,7 +1061,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" s="8"/>
       <c r="B13" t="s">
         <v>38</v>
@@ -1070,7 +1076,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1086,7 +1092,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1109,7 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1113,7 +1119,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="2"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>

</xml_diff>